<commit_message>
Revised data mapping and added resources folder
</commit_message>
<xml_diff>
--- a/Movies_Data_Mapping.xlsx
+++ b/Movies_Data_Mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Desktop\Bootcamp\Project\project 2 data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Desktop\Bootcamp\Project\project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F09ABD-CB7A-49DC-B465-57A64E777756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AF4FCE-4E82-48DE-9674-5271F5675D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{06870EEF-AC2F-4F30-9147-FBE95D58FC39}"/>
   </bookViews>
@@ -48,27 +48,15 @@
     <t>Source Datatype</t>
   </si>
   <si>
-    <t>Source DB</t>
-  </si>
-  <si>
-    <t>file</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
-    <t>target_db</t>
-  </si>
-  <si>
     <t>Business Rule</t>
   </si>
   <si>
-    <t>imdb.txt</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -79,9 +67,6 @@
   </si>
   <si>
     <t>imdb</t>
-  </si>
-  <si>
-    <t>netflix.txt</t>
   </si>
   <si>
     <t>netflix</t>
@@ -156,6 +141,21 @@
   </si>
   <si>
     <t>float</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>movies_db</t>
+  </si>
+  <si>
+    <t>netflix_title.csv</t>
+  </si>
+  <si>
+    <t>IMDb movies.csv</t>
+  </si>
+  <si>
+    <t>Source File</t>
   </si>
 </sst>
 </file>
@@ -528,16 +528,16 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
@@ -547,7 +547,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -573,33 +573,33 @@
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -607,28 +607,28 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
       <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
       <c r="I3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K3">
         <v>3</v>
@@ -636,28 +636,28 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K4">
         <v>2</v>
@@ -665,28 +665,28 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K5">
         <v>3</v>
@@ -694,28 +694,28 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="H6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
       <c r="I6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -723,28 +723,28 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
         <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" t="s">
-        <v>27</v>
       </c>
       <c r="K7">
         <v>3</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -768,7 +768,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -776,7 +776,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>